<commit_message>
update avta course excel files
</commit_message>
<xml_diff>
--- a/courses/excel/offshore/region-1/avta/FACULTY_OF_BUSINESS_AND_TECHNOLOGY.xlsx
+++ b/courses/excel/offshore/region-1/avta/FACULTY_OF_BUSINESS_AND_TECHNOLOGY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aibtaus-my.sharepoint.com/personal/f_zhang_aibtglobal_edu_au/Documents/App for VC/excel table template/Excel For New School AVTA/onshore/coe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aibtaus-my.sharepoint.com/personal/f_zhang_aibtglobal_edu_au/Documents/App for VC/excel table template/Excel For New School AVTA Course Added/offshore/Region3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_8B0793BCA77FB21812844C3ABEBA72B099DE0730" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F7BA76B-4E9F-411A-9679-741BC3E71A95}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="11_8B0793BCA77FB21812844C3ABEBA72B099DE0730" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7C056D7-4F71-4B27-8346-F2E0F69F3FAD}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-7710" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>vetCode</t>
   </si>
@@ -81,6 +81,70 @@
   <si>
     <t>promotionValidity</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIPLOMA OF CIVIL CONSTRUCTION DESIGN</t>
+  </si>
+  <si>
+    <t>44 wks Tuition + 8 wks Break</t>
+  </si>
+  <si>
+    <t>TAS</t>
+  </si>
+  <si>
+    <t>ADVANCED DIPLOMA OF CIVIL CONSTRUCTION DESIGN</t>
+  </si>
+  <si>
+    <t>111826A</t>
+  </si>
+  <si>
+    <t>RII60520</t>
+  </si>
+  <si>
+    <t>88 wks tuition + 16 wks break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADVANCED DIPLOMA OF INFORMATION TECHNOLOGY 
+(TELECOMMUNICATIONS NETWORK ENGINEERING) </t>
+  </si>
+  <si>
+    <t>ICT60220</t>
+  </si>
+  <si>
+    <t>111825B</t>
+  </si>
+  <si>
+    <t>PACKAGES</t>
+  </si>
+  <si>
+    <t>DIPLOMA OF CIVIL CONSTRUCTION DESIGN + ADVANCED DIPLOMA OF CIVIL CONSTRUCTION DESIGN</t>
+  </si>
+  <si>
+    <t>RII50520/RII60520</t>
+  </si>
+  <si>
+    <t>111827M/111826A</t>
+  </si>
+  <si>
+    <t>CIVIL CONSTRUCTION DESIGN</t>
+  </si>
+  <si>
+    <t>INFORMATION TECHNOLOGY</t>
+  </si>
+  <si>
+    <t>19,000 tuition fee + 200 handling fee</t>
+  </si>
+  <si>
+    <t>29,000 tuition fee + 200 handling fee</t>
+  </si>
+  <si>
+    <t>14,000 tuition fee + 200 handling fee</t>
+  </si>
+  <si>
+    <t>RII50520</t>
+  </si>
+  <si>
+    <t>111827M</t>
   </si>
 </sst>
 </file>
@@ -131,12 +195,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -419,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD23"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -502,8 +570,122 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" ht="45">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>52</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="3">
+        <v>19200</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
       <c r="R2" s="2"/>
+    </row>
+    <row r="3" spans="1:18" ht="45">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>104</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3">
+        <v>29200</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="45">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>104</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="3">
+        <v>14200</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="45">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5">
+        <v>104</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3">
+        <v>29200</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>